<commit_message>
I'm really fucked up with naming
</commit_message>
<xml_diff>
--- a/name.xlsx
+++ b/name.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3090" yWindow="510" windowWidth="15375" windowHeight="9825" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="09thAug, 2021" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy\ mmm\ dd"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -395,15 +396,97 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BARKAT</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>44411.92357494213</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>44411.92362424768</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44411.92367181713</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>44415.85362371528</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>44415.8536778125</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>44415.85373260417</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>44415.85535320602</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>44415.85540259259</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>44415.85607518518</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n">
+        <v>58.33856803844867</v>
+      </c>
+      <c r="C3" t="n">
+        <v>57.62532045244792</v>
+      </c>
+      <c r="D3" t="n">
+        <v>52.69172523621466</v>
+      </c>
+      <c r="E3" t="n">
+        <v>65.61309250155279</v>
+      </c>
+      <c r="F3" t="n">
+        <v>59.45638265356536</v>
+      </c>
+      <c r="G3" t="n">
+        <v>59.64865442257383</v>
+      </c>
+      <c r="H3" t="n">
+        <v>61.89463967501755</v>
+      </c>
+      <c r="I3" t="n">
+        <v>66.89636435307966</v>
+      </c>
+      <c r="J3" t="n">
+        <v>55.75754485861658</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:AF7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="18.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="32" max="32"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -412,24 +495,193 @@
           <t>BARKAT</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>56.54406461793793</v>
+      <c r="B2" s="1" t="n">
+        <v>44417.82224016204</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44408.98564814815</v>
+        <v>44417.82229238426</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>44417.82234395833</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>44417.82239103009</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>44417.82244174769</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>44417.82248809028</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>44417.82254042824</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>44417.82258753472</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>44417.82263921297</v>
+      </c>
+      <c r="K2" s="1" t="n">
+        <v>44417.82268840278</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>44417.82273489583</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>44417.82280960648</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>44417.82288429398</v>
+      </c>
+      <c r="O2" s="1" t="n">
+        <v>44417.82293166667</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>44417.82298355324</v>
+      </c>
+      <c r="Q2" s="1" t="n">
+        <v>44417.8230332176</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>44417.82308399305</v>
+      </c>
+      <c r="S2" s="1" t="n">
+        <v>44417.82313601852</v>
+      </c>
+      <c r="T2" s="1" t="n">
+        <v>44417.82358487268</v>
+      </c>
+      <c r="U2" s="1" t="n">
+        <v>44417.8236327199</v>
+      </c>
+      <c r="V2" s="1" t="n">
+        <v>44417.82368076389</v>
+      </c>
+      <c r="W2" s="1" t="n">
+        <v>44417.82373652777</v>
+      </c>
+      <c r="X2" s="1" t="n">
+        <v>44417.82395400463</v>
+      </c>
+      <c r="Y2" s="1" t="n">
+        <v>44417.82400850694</v>
+      </c>
+      <c r="Z2" s="1" t="n">
+        <v>44417.82405871528</v>
+      </c>
+      <c r="AA2" s="1" t="n">
+        <v>44417.94652545139</v>
+      </c>
+      <c r="AB2" s="1" t="n">
+        <v>44417.94657619213</v>
+      </c>
+      <c r="AC2" s="1" t="n">
+        <v>44417.94662560185</v>
+      </c>
+      <c r="AD2" s="1" t="n">
+        <v>44417.94667478009</v>
+      </c>
+      <c r="AE2" s="1" t="n">
+        <v>44417.94672203704</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>44417.94677083333</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DIP</t>
-        </is>
-      </c>
       <c r="B3" t="n">
-        <v>74.27852406959478</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>44408.98594118056</v>
+        <v>53.542823658927</v>
+      </c>
+      <c r="C3" t="n">
+        <v>60.36523559205251</v>
+      </c>
+      <c r="D3" t="n">
+        <v>56.96394311889464</v>
+      </c>
+      <c r="E3" t="n">
+        <v>54.72813178449628</v>
+      </c>
+      <c r="F3" t="n">
+        <v>55.40253417910125</v>
+      </c>
+      <c r="G3" t="n">
+        <v>57.24940752368606</v>
+      </c>
+      <c r="H3" t="n">
+        <v>57.62825205617263</v>
+      </c>
+      <c r="I3" t="n">
+        <v>56.81970962492681</v>
+      </c>
+      <c r="J3" t="n">
+        <v>55.29277788015965</v>
+      </c>
+      <c r="K3" t="n">
+        <v>54.14678840136179</v>
+      </c>
+      <c r="L3" t="n">
+        <v>54.85523509095866</v>
+      </c>
+      <c r="M3" t="n">
+        <v>59.85810148883542</v>
+      </c>
+      <c r="N3" t="n">
+        <v>61.86370041331051</v>
+      </c>
+      <c r="O3" t="n">
+        <v>54.51973910703432</v>
+      </c>
+      <c r="P3" t="n">
+        <v>53.72616683470605</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>53.31724502116864</v>
+      </c>
+      <c r="R3" t="n">
+        <v>50.85847973388519</v>
+      </c>
+      <c r="S3" t="n">
+        <v>57.8340071878003</v>
+      </c>
+      <c r="T3" t="n">
+        <v>53.05560272653313</v>
+      </c>
+      <c r="U3" t="n">
+        <v>57.62913473415546</v>
+      </c>
+      <c r="V3" t="n">
+        <v>52.92641729173631</v>
+      </c>
+      <c r="W3" t="n">
+        <v>56.08790410098113</v>
+      </c>
+      <c r="X3" t="n">
+        <v>55.48319966925911</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>52.50968075018424</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>60.34213673823531</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>54.56749361951794</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>50.13678485008185</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>51.97028951994359</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>50.58696131401567</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>53.84506514160032</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>57.89640483625501</v>
       </c>
     </row>
     <row r="4">
@@ -438,14 +690,73 @@
           <t>PARTHO</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>52.57315758720868</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>44408.98693019676</v>
+      <c r="B4" s="1" t="n">
+        <v>44417.82328145833</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>44417.82334966435</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>44417.82340376158</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>44417.82345313657</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>44417.82350561343</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>44417.82355653936</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>67.55517600591367</v>
+      </c>
+      <c r="C5" t="n">
+        <v>63.4348087892302</v>
+      </c>
+      <c r="D5" t="n">
+        <v>72.91781515037208</v>
+      </c>
+      <c r="E5" t="n">
+        <v>69.04050218910706</v>
+      </c>
+      <c r="F5" t="n">
+        <v>67.51575826061158</v>
+      </c>
+      <c r="G5" t="n">
+        <v>67.60920205228281</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>DIP</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>44417.82379689815</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>44417.82385122685</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>44417.82390922453</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n">
+        <v>74.92791161028117</v>
+      </c>
+      <c r="C7" t="n">
+        <v>75.14010206192152</v>
+      </c>
+      <c r="D7" t="n">
+        <v>70.049043613039</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>